<commit_message>
Goal.PercentComplete is working correctly for PercentGoalTasks.
</commit_message>
<xml_diff>
--- a/Design/Weighted Progress.xlsx
+++ b/Design/Weighted Progress.xlsx
@@ -5,15 +5,14 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Code\GitHub\SmartSession\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Personal\Code\GitHub\SmartSession\Design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
-    <sheet name="Revised" sheetId="2" r:id="rId1"/>
-    <sheet name="Initial" sheetId="1" r:id="rId2"/>
+    <sheet name="Current Calculation" sheetId="5" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,18 +23,94 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Rob Blake</author>
+  </authors>
+  <commentList>
+    <comment ref="E5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E12" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E25" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
   <si>
     <t>Task</t>
   </si>
   <si>
-    <t>Percent Progress</t>
-  </si>
-  <si>
-    <t>Weighting</t>
-  </si>
-  <si>
     <t>Total Progress</t>
   </si>
   <si>
@@ -51,20 +126,38 @@
     <t>Task 4</t>
   </si>
   <si>
-    <t>Weighted Value</t>
-  </si>
-  <si>
-    <t>Weighting (%)</t>
-  </si>
-  <si>
     <t>Percent Progress (%)</t>
+  </si>
+  <si>
+    <t>Weighting (Property)</t>
+  </si>
+  <si>
+    <t>Calc. Slice of Pie</t>
+  </si>
+  <si>
+    <t>Weighted %</t>
+  </si>
+  <si>
+    <t>Task 5</t>
+  </si>
+  <si>
+    <t>Task 6</t>
+  </si>
+  <si>
+    <t>Task 7</t>
+  </si>
+  <si>
+    <t>Task 8</t>
+  </si>
+  <si>
+    <t>Task 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -80,8 +173,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -100,22 +206,19 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -142,14 +245,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -429,213 +531,442 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="57.7109375" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="3" max="3" width="32.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="25.28515625" customWidth="1"/>
+    <col min="5" max="5" width="20.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2">
+        <v>100</v>
+      </c>
+      <c r="D2">
+        <v>6000</v>
+      </c>
+      <c r="E2">
+        <f xml:space="preserve"> (D2 / SUM(D2:D4)) * 100</f>
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <f>(C2 / 100) * E2</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="2">
+        <v>60</v>
+      </c>
+      <c r="D3">
+        <v>12000</v>
+      </c>
+      <c r="E3">
+        <f xml:space="preserve"> (D3 / SUM(D2:D4)) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="F3">
+        <f>(C3 / 100) * E3</f>
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="C4" s="2">
+        <v>25</v>
+      </c>
+      <c r="D4">
+        <v>6000</v>
+      </c>
+      <c r="E4">
+        <f xml:space="preserve"> (D4 / SUM(D2:D4)) * 100</f>
+        <v>25</v>
+      </c>
+      <c r="F4">
+        <f>(C4 / 100) * E4</f>
+        <v>6.25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C5" s="3"/>
+      <c r="E5" s="1">
+        <f>SUM(E2:E4)</f>
+        <v>100</v>
+      </c>
+      <c r="F5" s="5">
+        <f>SUM(F2:F4)</f>
+        <v>61.25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8" s="2">
+        <v>100</v>
+      </c>
+      <c r="D8">
+        <v>25</v>
+      </c>
+      <c r="E8">
+        <f xml:space="preserve"> (D8 / SUM(D8:D11)) * 100</f>
+        <v>12.5</v>
+      </c>
+      <c r="F8">
+        <f>(C8 / 100) * E8</f>
+        <v>12.5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="2">
+        <v>60</v>
+      </c>
+      <c r="D9">
+        <v>40</v>
+      </c>
+      <c r="E9">
+        <f xml:space="preserve"> (D9 / SUM(D8:D11)) * 100</f>
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <f>(C9 / 100) * E9</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>4</v>
+      </c>
+      <c r="C10" s="2">
+        <v>40</v>
+      </c>
+      <c r="D10">
+        <v>60</v>
+      </c>
+      <c r="E10">
+        <f xml:space="preserve"> (D10 / SUM(D8:D12)) * 100</f>
+        <v>30</v>
+      </c>
+      <c r="F10">
+        <f>(C10 / 100) * E10</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2">
+        <v>25</v>
+      </c>
+      <c r="D11">
+        <v>75</v>
+      </c>
+      <c r="E11">
+        <f xml:space="preserve"> (D11 / SUM(D8:D11)) * 100</f>
+        <v>37.5</v>
+      </c>
+      <c r="F11">
+        <f>(C11 / 100) * E11</f>
+        <v>9.375</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C12" s="3"/>
+      <c r="E12" s="1">
+        <f>SUM(E8:E11)</f>
+        <v>100</v>
+      </c>
+      <c r="F12" s="5">
+        <f>SUM(F8:F11)</f>
+        <v>45.875</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>2</v>
+      </c>
+      <c r="C15" s="2">
+        <v>100</v>
+      </c>
+      <c r="D15">
+        <v>25</v>
+      </c>
+      <c r="E15">
+        <f xml:space="preserve"> (D15 / SUM(D15:D24)) * 100</f>
+        <v>5</v>
+      </c>
+      <c r="F15">
+        <f>(C15 / 100) * E15</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>3</v>
+      </c>
+      <c r="C16" s="2">
+        <v>100</v>
+      </c>
+      <c r="D16">
+        <v>40</v>
+      </c>
+      <c r="E16">
+        <f xml:space="preserve"> (D16 / SUM(D15:D24)) * 100</f>
+        <v>8</v>
+      </c>
+      <c r="F16">
+        <f>(C16 / 100) * E16</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C17" s="2">
+        <v>100</v>
+      </c>
+      <c r="D17">
+        <v>60</v>
+      </c>
+      <c r="E17">
+        <f xml:space="preserve"> (D17 / SUM(D15:D24)) * 100</f>
+        <v>12</v>
+      </c>
+      <c r="F17">
+        <f>(C17 / 100) * E17</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>5</v>
+      </c>
+      <c r="C18" s="2">
+        <v>100</v>
+      </c>
+      <c r="D18">
+        <v>40</v>
+      </c>
+      <c r="E18">
+        <f xml:space="preserve"> (D18 / SUM(D15:D24)) * 100</f>
+        <v>8</v>
+      </c>
+      <c r="F18">
+        <f>(C18 / 100) * E18</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
         <v>10</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>30</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C2 / 100)</f>
-        <v>7.5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
+      <c r="C19" s="2">
+        <v>100</v>
+      </c>
+      <c r="D19">
         <v>60</v>
       </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C3 / 100)</f>
+      <c r="E19">
+        <f xml:space="preserve"> (D19 / SUM(D15:D24)) * 100</f>
+        <v>12</v>
+      </c>
+      <c r="F19">
+        <f>(C19 / 100) * E19</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>3</v>
+      </c>
+      <c r="C20" s="2">
+        <v>100</v>
+      </c>
+      <c r="D20">
+        <v>40</v>
+      </c>
+      <c r="E20">
+        <f xml:space="preserve"> (D20 / SUM(D15:D24)) * 100</f>
+        <v>8</v>
+      </c>
+      <c r="F20">
+        <f>(C20 / 100) * E20</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="2">
+        <v>100</v>
+      </c>
+      <c r="D21">
+        <v>60</v>
+      </c>
+      <c r="E21">
+        <f xml:space="preserve"> (D21 / SUM(D15:D24)) * 100</f>
+        <v>12</v>
+      </c>
+      <c r="F21">
+        <f>(C21 / 100) * E21</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>12</v>
+      </c>
+      <c r="C22" s="2">
+        <v>100</v>
+      </c>
+      <c r="D22">
+        <v>40</v>
+      </c>
+      <c r="E22">
+        <f xml:space="preserve"> (D22 / SUM(D15:D24)) * 100</f>
+        <v>8</v>
+      </c>
+      <c r="F22">
+        <f>(C22 / 100) * E22</f>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" s="2">
+        <v>100</v>
+      </c>
+      <c r="D23">
+        <v>60</v>
+      </c>
+      <c r="E23">
+        <f xml:space="preserve"> (D23 / SUM(D15:D24)) * 100</f>
+        <v>12</v>
+      </c>
+      <c r="F23">
+        <f>(C23 / 100) * E23</f>
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="2">
+        <v>100</v>
+      </c>
+      <c r="D24">
+        <v>75</v>
+      </c>
+      <c r="E24">
+        <f xml:space="preserve"> (D24 / SUM(D15:D24)) * 100</f>
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>15.2</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-      <c r="E4">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C4 / 100)</f>
-        <v>3.8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>68</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C5 / 100)</f>
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5">
-        <f>SUM(E2:E5)</f>
-        <v>43.3</v>
+      <c r="F24">
+        <f>(C24 / 100) * E24</f>
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C25" s="3"/>
+      <c r="E25" s="1">
+        <f>SUM(E15:E24)</f>
+        <v>100</v>
+      </c>
+      <c r="F25" s="5">
+        <f>SUM(F15:F24)</f>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E6"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="57.7109375" customWidth="1"/>
-    <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="32.140625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="5" width="16" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:5" s="6" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="6" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="6" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" s="3">
-        <v>100</v>
-      </c>
-      <c r="D2">
-        <v>5</v>
-      </c>
-      <c r="E2">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C2 / 100)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="3">
-        <v>100</v>
-      </c>
-      <c r="D3">
-        <v>65</v>
-      </c>
-      <c r="E3">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C3 / 100)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="3">
-        <v>100</v>
-      </c>
-      <c r="D4">
-        <v>25</v>
-      </c>
-      <c r="E4">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C4 / 100)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="4">
-        <v>100</v>
-      </c>
-      <c r="D5" s="1">
-        <v>5</v>
-      </c>
-      <c r="E5">
-        <f xml:space="preserve"> (SUM(D2:D5) / 4) * (C5 / 100)</f>
-        <v>25</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5">
-        <f>SUM(E2:E5)</f>
-        <v>100</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added some more weighted progress excel calculation rules.
</commit_message>
<xml_diff>
--- a/Design/Weighted Progress.xlsx
+++ b/Design/Weighted Progress.xlsx
@@ -101,12 +101,108 @@
         </r>
       </text>
     </comment>
+    <comment ref="E30" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E35" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E40" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E45" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Rob Blake:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Sum of the values in this row should always be = to 100%. Since we're calculating the % of the pie that each task can contribute to….</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
   <si>
     <t>Task</t>
   </si>
@@ -151,6 +247,15 @@
   </si>
   <si>
     <t>Task 9</t>
+  </si>
+  <si>
+    <t>Metronome Speed</t>
+  </si>
+  <si>
+    <t>Time Practiced</t>
+  </si>
+  <si>
+    <t>Exercise Weighted Progress</t>
   </si>
 </sst>
 </file>
@@ -532,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A49" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,7 +880,7 @@
         <v>5</v>
       </c>
       <c r="F15">
-        <f>(C15 / 100) * E15</f>
+        <f t="shared" ref="F15:F24" si="0">(C15 / 100) * E15</f>
         <v>5</v>
       </c>
     </row>
@@ -794,7 +899,7 @@
         <v>8</v>
       </c>
       <c r="F16">
-        <f>(C16 / 100) * E16</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -813,7 +918,7 @@
         <v>12</v>
       </c>
       <c r="F17">
-        <f>(C17 / 100) * E17</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -832,7 +937,7 @@
         <v>8</v>
       </c>
       <c r="F18">
-        <f>(C18 / 100) * E18</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -851,7 +956,7 @@
         <v>12</v>
       </c>
       <c r="F19">
-        <f>(C19 / 100) * E19</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -870,7 +975,7 @@
         <v>8</v>
       </c>
       <c r="F20">
-        <f>(C20 / 100) * E20</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -889,7 +994,7 @@
         <v>12</v>
       </c>
       <c r="F21">
-        <f>(C21 / 100) * E21</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -908,7 +1013,7 @@
         <v>8</v>
       </c>
       <c r="F22">
-        <f>(C22 / 100) * E22</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
     </row>
@@ -927,7 +1032,7 @@
         <v>12</v>
       </c>
       <c r="F23">
-        <f>(C23 / 100) * E23</f>
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
     </row>
@@ -946,7 +1051,7 @@
         <v>15</v>
       </c>
       <c r="F24">
-        <f>(C24 / 100) * E24</f>
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
     </row>
@@ -962,6 +1067,282 @@
       <c r="F25" s="5">
         <f>SUM(F15:F24)</f>
         <v>100</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>15</v>
+      </c>
+      <c r="C28" s="2">
+        <v>100</v>
+      </c>
+      <c r="D28">
+        <v>6000</v>
+      </c>
+      <c r="E28">
+        <f xml:space="preserve"> (D28 / SUM(D28:D29)) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="F28">
+        <f>(C28 / 100) * E28</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C29" s="2">
+        <v>50</v>
+      </c>
+      <c r="D29">
+        <v>6000</v>
+      </c>
+      <c r="E29">
+        <f xml:space="preserve"> (D29 / SUM(D28:D29)) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="F29">
+        <f>(C29 / 100) * E29</f>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="E30" s="1">
+        <f>SUM(E28:E29)</f>
+        <v>100</v>
+      </c>
+      <c r="F30" s="5">
+        <f>SUM(F28:F29)</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E32" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>15</v>
+      </c>
+      <c r="C33" s="2">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <f xml:space="preserve"> (D33 / SUM(D33:D34)) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <f>(C33 / 100) * E33</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>16</v>
+      </c>
+      <c r="C34" s="2">
+        <v>50</v>
+      </c>
+      <c r="D34">
+        <v>6000</v>
+      </c>
+      <c r="E34">
+        <f xml:space="preserve"> (D34 / SUM(D33:D34)) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="F34">
+        <f>(C34 / 100) * E34</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="E35" s="1">
+        <f>SUM(E33:E34)</f>
+        <v>100</v>
+      </c>
+      <c r="F35" s="5">
+        <f>SUM(F33:F34)</f>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F37" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>15</v>
+      </c>
+      <c r="C38" s="2">
+        <v>100</v>
+      </c>
+      <c r="D38">
+        <v>6000</v>
+      </c>
+      <c r="E38">
+        <f xml:space="preserve"> (D38 / SUM(D38:D39)) * 100</f>
+        <v>100</v>
+      </c>
+      <c r="F38">
+        <f>(C38 / 100) * E38</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>16</v>
+      </c>
+      <c r="C39" s="2">
+        <v>50</v>
+      </c>
+      <c r="D39">
+        <v>0</v>
+      </c>
+      <c r="E39">
+        <f xml:space="preserve"> (D39 / SUM(D38:D39)) * 100</f>
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <f>(C39 / 100) * E39</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C40" s="3"/>
+      <c r="E40" s="1">
+        <f>SUM(E38:E39)</f>
+        <v>100</v>
+      </c>
+      <c r="F40" s="5">
+        <f>SUM(F38:F39)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" s="4" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A42" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>15</v>
+      </c>
+      <c r="C43" s="2">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>50</v>
+      </c>
+      <c r="E43">
+        <f xml:space="preserve"> (D43 / SUM(D43:D44)) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="F43">
+        <f>(C43 / 100) * E43</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>16</v>
+      </c>
+      <c r="C44" s="2">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>50</v>
+      </c>
+      <c r="E44">
+        <f xml:space="preserve"> (D44 / SUM(D43:D44)) * 100</f>
+        <v>50</v>
+      </c>
+      <c r="F44">
+        <f>(C44 / 100) * E44</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C45" s="3"/>
+      <c r="E45" s="1">
+        <f>SUM(E43:E44)</f>
+        <v>100</v>
+      </c>
+      <c r="F45" s="5">
+        <f>SUM(F43:F44)</f>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>